<commit_message>
add create table sql
</commit_message>
<xml_diff>
--- a/dom/DB定義書.xlsx
+++ b/dom/DB定義書.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://faulkneracademyorg-my.sharepoint.com/personal/g27879_y365_me/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t-bli/workspace/stsystem/dom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="8_{4DE37044-8FE1-7F4E-A874-41355F4A9F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DDA7F3E-BC5A-0949-AAB3-271D2D953EBF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E58CE5C-6F2B-DC47-BA8C-40AD9B76284F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="3" xr2:uid="{F53B2AFE-26CF-1F41-8AC4-0066847C8E6C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="108">
   <si>
     <t>ST_システム</t>
     <phoneticPr fontId="1"/>
@@ -254,10 +254,6 @@
   </si>
   <si>
     <t>CREATE_USER</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>string</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1308,6 +1304,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1317,116 +1358,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1748,7 +1744,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16:Q16"/>
+      <selection activeCell="L12" sqref="L12:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1763,58 +1759,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="22" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="53" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="53" t="s">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="53" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="53" t="s">
+      <c r="Q1" s="38"/>
+      <c r="R1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="60"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" s="22" customFormat="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="61"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="7" customHeight="1">
       <c r="A3" s="15"/>
@@ -1839,16 +1835,16 @@
     </row>
     <row r="4" spans="1:19" s="18" customFormat="1">
       <c r="A4" s="19"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -1864,16 +1860,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="8"/>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1891,20 +1887,20 @@
       <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="62"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="25" t="s">
         <v>9</v>
       </c>
@@ -1917,66 +1913,66 @@
       <c r="M6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="65"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="55"/>
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="31"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="62"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="48" t="s">
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="51"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="27">
         <v>8</v>
       </c>
@@ -1987,31 +1983,31 @@
         <v>24</v>
       </c>
       <c r="M8" s="27"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="31"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="62"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="34" t="s">
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="I9" s="44"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="56"/>
       <c r="J9" s="3" t="s">
         <v>26</v>
       </c>
@@ -2022,31 +2018,31 @@
         <v>24</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="63"/>
     </row>
     <row r="10" spans="1:19" ht="67" customHeight="1">
       <c r="A10" s="10">
         <v>4</v>
       </c>
-      <c r="B10" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="48" t="s">
+      <c r="B10" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="50"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="51"/>
+      <c r="I10" s="61"/>
       <c r="J10" s="3">
         <v>1</v>
       </c>
@@ -2057,33 +2053,33 @@
         <v>24</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="O10" s="49"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="42"/>
+      <c r="N10" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="64"/>
+      <c r="S10" s="65"/>
     </row>
     <row r="11" spans="1:19" ht="41" customHeight="1">
       <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="34" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="44"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="3">
         <v>1</v>
       </c>
@@ -2094,194 +2090,202 @@
         <v>24</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N11" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="N11" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="34" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="34" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="3"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="L12" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M12" s="3"/>
-      <c r="N12" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
+      <c r="N12" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="63"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="10">
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="34" t="s">
+      <c r="B13" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="28" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="43"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="3">
         <v>8</v>
       </c>
       <c r="K13" s="5">
         <v>8</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="35"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="45" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="46"/>
+      <c r="I14" s="58"/>
       <c r="J14" s="3"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="35"/>
+      <c r="N14" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="10">
         <v>9</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="28" t="s">
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="43"/>
+      <c r="I15" s="55"/>
       <c r="J15" s="3">
         <v>8</v>
       </c>
       <c r="K15" s="5">
         <v>8</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="35"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="10">
         <v>10</v>
       </c>
-      <c r="B16" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="34" t="s">
+      <c r="B16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="45" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="46"/>
+      <c r="I16" s="58"/>
       <c r="J16" s="3"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
+      <c r="N16" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="63"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="10">
         <v>11</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="28" t="s">
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="43"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="3">
         <v>8</v>
       </c>
@@ -2290,49 +2294,82 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19" ht="21" thickBot="1">
       <c r="A18" s="12"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="47"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="59"/>
       <c r="J18" s="13"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="33"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:J2"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
@@ -2349,52 +2386,19 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="N10:Q10"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:J2"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="N1:O2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2407,7 +2411,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21:Q21"/>
+      <selection activeCell="L18" sqref="L18:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2422,58 +2426,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="22" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="53" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="53" t="s">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="53" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="53" t="s">
+      <c r="Q1" s="38"/>
+      <c r="R1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="60"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" s="22" customFormat="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="61"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="7" customHeight="1">
       <c r="A3" s="15"/>
@@ -2498,16 +2502,16 @@
     </row>
     <row r="4" spans="1:19" s="18" customFormat="1">
       <c r="A4" s="19"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -2523,16 +2527,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="8"/>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2550,20 +2554,20 @@
       <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="62"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="25" t="s">
         <v>9</v>
       </c>
@@ -2576,132 +2580,132 @@
       <c r="M6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="65"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="43"/>
+      <c r="B7" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="55"/>
       <c r="J7" s="2"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="31"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="62"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="34" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="43"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="55"/>
       <c r="J8" s="6"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M8" s="7"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="35"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="63"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="34" t="s">
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="56"/>
+      <c r="J9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="44"/>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="63"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="10">
         <v>4</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="44"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="56"/>
       <c r="J10" s="3">
         <v>2</v>
       </c>
@@ -2712,31 +2716,31 @@
         <v>24</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="35"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="63"/>
     </row>
     <row r="11" spans="1:19" ht="39" customHeight="1">
       <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="34" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="44"/>
+      <c r="I11" s="56"/>
       <c r="J11" s="3">
         <v>1</v>
       </c>
@@ -2745,33 +2749,33 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="35"/>
+      <c r="N11" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="34" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="3">
         <v>13</v>
       </c>
@@ -2780,62 +2784,66 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
+      <c r="N12" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="63"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="10">
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" s="44"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="5"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="56"/>
+      <c r="J13" s="3">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5">
+        <v>50</v>
+      </c>
       <c r="L13" s="5"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="35"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:19" ht="59" customHeight="1">
       <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="44"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="56"/>
       <c r="J14" s="3">
         <v>1</v>
       </c>
@@ -2846,33 +2854,33 @@
         <v>24</v>
       </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="35"/>
+      <c r="N14" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="10">
         <v>9</v>
       </c>
-      <c r="B15" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="44"/>
+      <c r="B15" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="56"/>
       <c r="J15" s="3">
         <v>2</v>
       </c>
@@ -2881,31 +2889,31 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="35"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="10">
         <v>10</v>
       </c>
-      <c r="B16" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="44"/>
+      <c r="B16" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="56"/>
       <c r="J16" s="3">
         <v>2</v>
       </c>
@@ -2914,31 +2922,31 @@
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="63"/>
     </row>
     <row r="17" spans="1:19" ht="41" customHeight="1">
       <c r="A17" s="10">
         <v>11</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="34" t="s">
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="44"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="3">
         <v>1</v>
       </c>
@@ -2949,194 +2957,202 @@
         <v>24</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N17" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="N17" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="10">
         <v>12</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="34" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="34" t="s">
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="44"/>
+      <c r="I18" s="56"/>
       <c r="J18" s="3"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M18" s="3"/>
-      <c r="N18" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="35"/>
+      <c r="N18" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="63"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="10">
         <v>13</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="34" t="s">
+      <c r="B19" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="28" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="43"/>
+      <c r="I19" s="55"/>
       <c r="J19" s="3">
         <v>8</v>
       </c>
       <c r="K19" s="5">
         <v>8</v>
       </c>
-      <c r="L19" s="5"/>
+      <c r="L19" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M19" s="3"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="35"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="63"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="10">
         <v>14</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="45" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="46"/>
+      <c r="I20" s="58"/>
       <c r="J20" s="3"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="L20" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="35"/>
+      <c r="N20" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="63"/>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="10">
         <v>15</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="28" t="s">
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="43"/>
+      <c r="I21" s="55"/>
       <c r="J21" s="3">
         <v>8</v>
       </c>
       <c r="K21" s="5">
         <v>8</v>
       </c>
-      <c r="L21" s="5"/>
+      <c r="L21" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M21" s="3"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="35"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="63"/>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="10">
         <v>16</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="34" t="s">
+      <c r="B22" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="45" t="s">
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="46"/>
+      <c r="I22" s="58"/>
       <c r="J22" s="3"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="35"/>
+      <c r="N22" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="63"/>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="10">
         <v>17</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="28" t="s">
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="43"/>
+      <c r="I23" s="55"/>
       <c r="J23" s="3">
         <v>8</v>
       </c>
@@ -3145,36 +3161,117 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="35"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="63"/>
     </row>
     <row r="24" spans="1:19" ht="21" thickBot="1">
       <c r="A24" s="12"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="47"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="59"/>
       <c r="J24" s="13"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="33"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="105">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="R1:S2"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:G8"/>
@@ -3199,90 +3296,10 @@
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="R24:S24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3291,7 +3308,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25:Q25"/>
+      <selection activeCell="L21" sqref="L21:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -3306,58 +3323,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="22" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="53" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="53" t="s">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="53" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="53" t="s">
+      <c r="Q1" s="38"/>
+      <c r="R1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="60"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" s="22" customFormat="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="61"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="7" customHeight="1">
       <c r="A3" s="15"/>
@@ -3382,16 +3399,16 @@
     </row>
     <row r="4" spans="1:19" s="18" customFormat="1">
       <c r="A4" s="19"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -3407,16 +3424,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="8"/>
-      <c r="B5" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52" t="s">
+      <c r="B5" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -3434,20 +3451,20 @@
       <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="62"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="25" t="s">
         <v>9</v>
       </c>
@@ -3460,163 +3477,163 @@
       <c r="M6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="65"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="43"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="55"/>
       <c r="J7" s="6"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="6"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="31"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="62"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="10">
         <v>2</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="28" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="55"/>
       <c r="J8" s="6"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="31"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="62"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="43"/>
+      <c r="B9" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="44"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="55"/>
       <c r="J9" s="6"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M9" s="6"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="31"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="62"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="10">
         <v>4</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="34" t="s">
+      <c r="B10" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="56"/>
+      <c r="J10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="44"/>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="35"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="63"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="44"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="56"/>
       <c r="J11" s="7">
         <v>2</v>
       </c>
@@ -3627,31 +3644,31 @@
         <v>24</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="35"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19" ht="39" customHeight="1">
       <c r="A12" s="10">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="34" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="7">
         <v>1</v>
       </c>
@@ -3660,33 +3677,33 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
+      <c r="N12" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="63"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="10">
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="34" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="44"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="7">
         <v>13</v>
       </c>
@@ -3695,62 +3712,62 @@
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="35"/>
+      <c r="N13" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="44"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="56"/>
       <c r="J14" s="7"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="35"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="10">
         <v>9</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="44"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="56"/>
       <c r="J15" s="7">
         <v>2</v>
       </c>
@@ -3759,31 +3776,31 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="35"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="10">
         <v>10</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="44"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="56"/>
       <c r="J16" s="7">
         <v>2</v>
       </c>
@@ -3792,31 +3809,31 @@
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="63"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="10">
         <v>11</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="34" t="s">
+      <c r="B17" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="44"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="7">
         <v>13</v>
       </c>
@@ -3825,95 +3842,95 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
+      <c r="N17" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="10">
         <v>12</v>
       </c>
-      <c r="B18" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I18" s="44"/>
+      <c r="B18" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="56"/>
       <c r="J18" s="7"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="35"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="63"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="10">
         <v>13</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="44"/>
+      <c r="B19" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="56"/>
       <c r="J19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="35"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="63"/>
     </row>
     <row r="20" spans="1:19" ht="41" customHeight="1">
       <c r="A20" s="10">
         <v>14</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="34" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="44"/>
+      <c r="I20" s="56"/>
       <c r="J20" s="7">
         <v>1</v>
       </c>
@@ -3924,194 +3941,202 @@
         <v>24</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N20" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="N20" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="63"/>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="10">
         <v>15</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="34" t="s">
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="34" t="s">
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I21" s="44"/>
+      <c r="I21" s="56"/>
       <c r="J21" s="7"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="L21" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M21" s="7"/>
-      <c r="N21" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="35"/>
+      <c r="N21" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="63"/>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="10">
         <v>16</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="34" t="s">
+      <c r="B22" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="28" t="s">
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="43"/>
+      <c r="I22" s="55"/>
       <c r="J22" s="7">
         <v>8</v>
       </c>
       <c r="K22" s="5">
         <v>8</v>
       </c>
-      <c r="L22" s="5"/>
+      <c r="L22" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M22" s="7"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="35"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="63"/>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="10">
         <v>17</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="45" t="s">
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="46"/>
+      <c r="I23" s="58"/>
       <c r="J23" s="7"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="L23" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M23" s="7"/>
-      <c r="N23" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="35"/>
+      <c r="N23" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="42"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="63"/>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="10">
         <v>18</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="28" t="s">
+      <c r="F24" s="41"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="43"/>
+      <c r="I24" s="55"/>
       <c r="J24" s="7">
         <v>8</v>
       </c>
       <c r="K24" s="5">
         <v>8</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M24" s="7"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="35"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="63"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="10">
         <v>19</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="34" t="s">
+      <c r="B25" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="45" t="s">
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="46"/>
+      <c r="I25" s="58"/>
       <c r="J25" s="7"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="35"/>
+      <c r="N25" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="63"/>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" s="10">
         <v>20</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="28" t="s">
+      <c r="F26" s="41"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="43"/>
+      <c r="I26" s="55"/>
       <c r="J26" s="7">
         <v>8</v>
       </c>
@@ -4120,46 +4145,122 @@
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="35"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="63"/>
     </row>
     <row r="27" spans="1:19" ht="21" thickBot="1">
       <c r="A27" s="12"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="47"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="59"/>
       <c r="J27" s="13"/>
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="13"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="33"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="120">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:J2"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:Q2"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="N23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="N24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="N25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="N26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N27:Q27"/>
+    <mergeCell ref="R27:S27"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="H17:I17"/>
@@ -4184,95 +4285,20 @@
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="N26:Q26"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="N27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="N24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="N23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="N21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:J2"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="R19:S19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4281,7 +4307,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4296,58 +4322,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="22" customFormat="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="53" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="53" t="s">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="53" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="53" t="s">
+      <c r="Q1" s="38"/>
+      <c r="R1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="60"/>
+      <c r="S1" s="29"/>
     </row>
     <row r="2" spans="1:19" s="22" customFormat="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="61"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="7" customHeight="1">
       <c r="A3" s="15"/>
@@ -4372,16 +4398,16 @@
     </row>
     <row r="4" spans="1:19" s="18" customFormat="1">
       <c r="A4" s="19"/>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -4397,16 +4423,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="8"/>
-      <c r="B5" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52" t="s">
+      <c r="B5" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4424,20 +4450,20 @@
       <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="62"/>
+      <c r="I6" s="32"/>
       <c r="J6" s="25" t="s">
         <v>9</v>
       </c>
@@ -4450,66 +4476,66 @@
       <c r="M6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="63" t="s">
+      <c r="N6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="S6" s="65"/>
+      <c r="S6" s="35"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="43"/>
+      <c r="B7" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="55"/>
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
       <c r="L7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="35"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="63"/>
     </row>
     <row r="8" spans="1:19" ht="63" customHeight="1">
       <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="28" t="s">
+      <c r="F8" s="44"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="43"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="2">
         <v>1</v>
       </c>
@@ -4521,32 +4547,32 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="31"/>
+        <v>50</v>
+      </c>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="62"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="11">
         <v>3</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="34" t="s">
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="44"/>
+      <c r="I9" s="56"/>
       <c r="J9" s="3">
         <v>8</v>
       </c>
@@ -4557,31 +4583,31 @@
         <v>24</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="63"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="11">
         <v>4</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="44"/>
+      <c r="B10" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="56"/>
       <c r="J10" s="3">
         <v>4</v>
       </c>
@@ -4592,31 +4618,31 @@
         <v>24</v>
       </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="35"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="63"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="11">
         <v>5</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="44"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="56"/>
       <c r="J11" s="3">
         <v>6</v>
       </c>
@@ -4627,31 +4653,31 @@
         <v>24</v>
       </c>
       <c r="M11" s="3"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="35"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="63"/>
     </row>
     <row r="12" spans="1:19" ht="41" customHeight="1">
       <c r="A12" s="11">
         <v>6</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="34" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="44"/>
+      <c r="I12" s="56"/>
       <c r="J12" s="3">
         <v>1</v>
       </c>
@@ -4662,194 +4688,204 @@
         <v>24</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N12" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
+        <v>58</v>
+      </c>
+      <c r="N12" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="63"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="11">
         <v>7</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="34" t="s">
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="34" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="44"/>
+      <c r="I13" s="56"/>
       <c r="J13" s="3"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="L13" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="35"/>
+      <c r="N13" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="63"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="11">
         <v>8</v>
       </c>
-      <c r="B14" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="34" t="s">
+      <c r="B14" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="28" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="43"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="3">
         <v>8</v>
       </c>
       <c r="K14" s="5">
         <v>8</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="35"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="11">
         <v>9</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="45" t="s">
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="46"/>
+      <c r="I15" s="58"/>
       <c r="J15" s="3"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="L15" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="35"/>
+      <c r="N15" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="11">
         <v>10</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="28" t="s">
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="43"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="3">
         <v>8</v>
       </c>
       <c r="K16" s="5">
         <v>8</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M16" s="3"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="63"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="11">
         <v>11</v>
       </c>
-      <c r="B17" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="34" t="s">
+      <c r="B17" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="45" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="46"/>
+      <c r="I17" s="58"/>
       <c r="J17" s="3"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="L17" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="M17" s="3"/>
-      <c r="N17" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
+      <c r="N17" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="11">
         <v>12</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="28" t="s">
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="43"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="3">
         <v>8</v>
       </c>
@@ -4858,48 +4894,91 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="35"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="63"/>
     </row>
     <row r="19" spans="1:19" ht="21" thickBot="1">
       <c r="A19" s="12"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="47"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="59"/>
       <c r="J19" s="13"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="33"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="52"/>
+      <c r="S19" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="R1:S2"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F1:J2"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="P1:Q2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="R6:S6"/>
@@ -4913,63 +4992,21 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="R7:S7"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="R1:S2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="F1:J2"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="P1:Q2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>